<commit_message>
Zeitplan und Doku fertig
</commit_message>
<xml_diff>
--- a/Zeitplanung.xlsx
+++ b/Zeitplanung.xlsx
@@ -159,7 +159,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="56">
   <si>
     <t>Nr.</t>
   </si>
@@ -325,14 +325,18 @@
   </si>
   <si>
     <t>Design</t>
+  </si>
+  <si>
+    <t>Ferien</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="26" x14ac:knownFonts="1">
     <font>
@@ -501,7 +505,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -575,6 +579,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -759,7 +769,7 @@
     </xf>
     <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -895,9 +905,6 @@
     <xf numFmtId="164" fontId="14" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="6" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -956,9 +963,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="11" xfId="3" applyBorder="1"/>
@@ -967,22 +971,67 @@
     <xf numFmtId="14" fontId="14" fillId="11" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="13" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="12" borderId="4" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="8" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="9" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="16" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="23" fillId="12" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="25" fillId="12" borderId="4" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="23" fillId="9" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="16" fillId="5" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="16" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="14" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1024,6 +1073,12 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Akzent2" xfId="5" builtinId="33"/>
@@ -1267,10 +1322,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5.5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>0</c:v>
@@ -1454,13 +1509,13 @@
                   <c:v>22.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1519,19 +1574,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>17.25</c:v>
+                  <c:v>19.75</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19.5</c:v>
+                  <c:v>22.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.5</c:v>
+                  <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>2</c:v>
@@ -2041,7 +2096,7 @@
   <dimension ref="A1:AP44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="AD34" sqref="AD34"/>
+      <selection activeCell="AE8" sqref="AE8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2059,40 +2114,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:42" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="99" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="86"/>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="86"/>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
-      <c r="I1" s="86"/>
-      <c r="J1" s="86"/>
-      <c r="K1" s="86"/>
-      <c r="L1" s="86"/>
-      <c r="M1" s="86"/>
-      <c r="N1" s="86"/>
-      <c r="O1" s="86"/>
-      <c r="P1" s="86"/>
-      <c r="Q1" s="86"/>
-      <c r="R1" s="86"/>
-      <c r="S1" s="86"/>
-      <c r="T1" s="86"/>
-      <c r="U1" s="86"/>
-      <c r="V1" s="86"/>
-      <c r="W1" s="86"/>
-      <c r="X1" s="86"/>
-      <c r="Y1" s="86"/>
-      <c r="Z1" s="86"/>
-      <c r="AA1" s="86"/>
-      <c r="AB1" s="86"/>
-      <c r="AC1" s="86"/>
-      <c r="AD1" s="86"/>
-      <c r="AE1" s="86"/>
-      <c r="AF1" s="86"/>
+      <c r="B1" s="99"/>
+      <c r="C1" s="99"/>
+      <c r="D1" s="99"/>
+      <c r="E1" s="99"/>
+      <c r="F1" s="99"/>
+      <c r="G1" s="99"/>
+      <c r="H1" s="99"/>
+      <c r="I1" s="99"/>
+      <c r="J1" s="99"/>
+      <c r="K1" s="99"/>
+      <c r="L1" s="99"/>
+      <c r="M1" s="99"/>
+      <c r="N1" s="99"/>
+      <c r="O1" s="99"/>
+      <c r="P1" s="99"/>
+      <c r="Q1" s="99"/>
+      <c r="R1" s="99"/>
+      <c r="S1" s="99"/>
+      <c r="T1" s="99"/>
+      <c r="U1" s="99"/>
+      <c r="V1" s="99"/>
+      <c r="W1" s="99"/>
+      <c r="X1" s="99"/>
+      <c r="Y1" s="99"/>
+      <c r="Z1" s="99"/>
+      <c r="AA1" s="99"/>
+      <c r="AB1" s="99"/>
+      <c r="AC1" s="99"/>
+      <c r="AD1" s="99"/>
+      <c r="AE1" s="99"/>
+      <c r="AF1" s="99"/>
       <c r="AG1" s="29"/>
       <c r="AH1" s="29"/>
       <c r="AI1" s="29"/>
@@ -2136,25 +2191,25 @@
       <c r="AC2" s="29"/>
       <c r="AD2" s="29"/>
       <c r="AE2" s="29"/>
-      <c r="AF2" s="67"/>
-      <c r="AG2" s="66"/>
-      <c r="AH2" s="66"/>
-      <c r="AI2" s="66"/>
-      <c r="AJ2" s="66"/>
-      <c r="AK2" s="66"/>
-      <c r="AL2" s="66"/>
-      <c r="AM2" s="66"/>
-      <c r="AN2" s="66"/>
-      <c r="AO2" s="66"/>
-      <c r="AP2" s="66"/>
+      <c r="AF2" s="66"/>
+      <c r="AG2" s="65"/>
+      <c r="AH2" s="65"/>
+      <c r="AI2" s="65"/>
+      <c r="AJ2" s="65"/>
+      <c r="AK2" s="65"/>
+      <c r="AL2" s="65"/>
+      <c r="AM2" s="65"/>
+      <c r="AN2" s="65"/>
+      <c r="AO2" s="65"/>
+      <c r="AP2" s="65"/>
     </row>
     <row r="3" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="34"/>
       <c r="B3" s="35"/>
-      <c r="C3" s="87" t="s">
+      <c r="C3" s="100" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="87"/>
+      <c r="D3" s="100"/>
       <c r="E3" s="34"/>
       <c r="F3" s="34"/>
       <c r="G3" s="34"/>
@@ -2162,45 +2217,45 @@
       <c r="I3" s="34"/>
       <c r="J3" s="34"/>
       <c r="K3" s="34"/>
-      <c r="L3" s="87" t="s">
+      <c r="L3" s="100" t="s">
         <v>23</v>
       </c>
-      <c r="M3" s="87"/>
-      <c r="N3" s="87"/>
-      <c r="O3" s="87"/>
-      <c r="P3" s="87"/>
-      <c r="Q3" s="87" t="s">
+      <c r="M3" s="100"/>
+      <c r="N3" s="100"/>
+      <c r="O3" s="100"/>
+      <c r="P3" s="100"/>
+      <c r="Q3" s="100" t="s">
         <v>24</v>
       </c>
-      <c r="R3" s="87"/>
-      <c r="S3" s="87"/>
-      <c r="T3" s="87"/>
-      <c r="U3" s="87"/>
-      <c r="V3" s="79"/>
-      <c r="W3" s="87" t="s">
+      <c r="R3" s="100"/>
+      <c r="S3" s="100"/>
+      <c r="T3" s="100"/>
+      <c r="U3" s="100"/>
+      <c r="V3" s="75"/>
+      <c r="W3" s="100" t="s">
         <v>25</v>
       </c>
-      <c r="X3" s="87"/>
-      <c r="Y3" s="87"/>
-      <c r="Z3" s="87"/>
-      <c r="AA3" s="87"/>
-      <c r="AB3" s="87" t="s">
+      <c r="X3" s="100"/>
+      <c r="Y3" s="100"/>
+      <c r="Z3" s="100"/>
+      <c r="AA3" s="100"/>
+      <c r="AB3" s="100" t="s">
         <v>26</v>
       </c>
-      <c r="AC3" s="87"/>
-      <c r="AD3" s="87"/>
-      <c r="AE3" s="87"/>
-      <c r="AF3" s="88"/>
-      <c r="AG3" s="81"/>
-      <c r="AH3" s="81"/>
-      <c r="AI3" s="81"/>
-      <c r="AJ3" s="81"/>
-      <c r="AK3" s="81"/>
-      <c r="AL3" s="81"/>
-      <c r="AM3" s="81"/>
-      <c r="AN3" s="81"/>
-      <c r="AO3" s="81"/>
-      <c r="AP3" s="81"/>
+      <c r="AC3" s="100"/>
+      <c r="AD3" s="100"/>
+      <c r="AE3" s="100"/>
+      <c r="AF3" s="101"/>
+      <c r="AG3" s="94"/>
+      <c r="AH3" s="94"/>
+      <c r="AI3" s="94"/>
+      <c r="AJ3" s="94"/>
+      <c r="AK3" s="94"/>
+      <c r="AL3" s="94"/>
+      <c r="AM3" s="94"/>
+      <c r="AN3" s="94"/>
+      <c r="AO3" s="94"/>
+      <c r="AP3" s="94"/>
     </row>
     <row r="4" spans="1:42" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="36" t="s">
@@ -2294,7 +2349,7 @@
       <c r="AE4" s="44">
         <v>43118</v>
       </c>
-      <c r="AF4" s="74"/>
+      <c r="AF4" s="72"/>
       <c r="AG4" s="27"/>
       <c r="AH4" s="27"/>
       <c r="AI4" s="27"/>
@@ -2319,7 +2374,7 @@
       </c>
       <c r="D5" s="25">
         <f>SUM(D6:D10)</f>
-        <v>17.25</v>
+        <v>19.75</v>
       </c>
       <c r="E5" s="30"/>
       <c r="F5" s="30"/>
@@ -2348,7 +2403,7 @@
       <c r="AC5" s="15"/>
       <c r="AD5" s="15"/>
       <c r="AE5" s="14"/>
-      <c r="AF5" s="71"/>
+      <c r="AF5" s="69"/>
     </row>
     <row r="6" spans="1:42" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="36">
@@ -2372,30 +2427,30 @@
       <c r="H6" s="47"/>
       <c r="I6" s="48"/>
       <c r="J6" s="36"/>
-      <c r="K6" s="49">
+      <c r="K6" s="82">
         <v>1</v>
       </c>
-      <c r="L6" s="50"/>
-      <c r="M6" s="50"/>
-      <c r="N6" s="51"/>
-      <c r="O6" s="51"/>
-      <c r="P6" s="51"/>
-      <c r="Q6" s="52"/>
-      <c r="R6" s="53"/>
-      <c r="S6" s="51"/>
+      <c r="L6" s="49"/>
+      <c r="M6" s="49"/>
+      <c r="N6" s="50"/>
+      <c r="O6" s="50"/>
+      <c r="P6" s="50"/>
+      <c r="Q6" s="51"/>
+      <c r="R6" s="52"/>
+      <c r="S6" s="50"/>
       <c r="T6" s="47"/>
-      <c r="U6" s="51"/>
-      <c r="V6" s="51"/>
-      <c r="W6" s="52"/>
-      <c r="X6" s="53"/>
-      <c r="Y6" s="51"/>
+      <c r="U6" s="50"/>
+      <c r="V6" s="91"/>
+      <c r="W6" s="51"/>
+      <c r="X6" s="52"/>
+      <c r="Y6" s="50"/>
       <c r="Z6" s="47"/>
-      <c r="AA6" s="51"/>
-      <c r="AB6" s="52"/>
-      <c r="AC6" s="53"/>
-      <c r="AD6" s="51"/>
-      <c r="AE6" s="69"/>
-      <c r="AF6" s="72"/>
+      <c r="AA6" s="50"/>
+      <c r="AB6" s="51"/>
+      <c r="AC6" s="52"/>
+      <c r="AD6" s="50"/>
+      <c r="AE6" s="68"/>
+      <c r="AF6" s="70"/>
       <c r="AG6" s="27"/>
       <c r="AH6" s="27"/>
       <c r="AI6" s="27"/>
@@ -2428,33 +2483,33 @@
       <c r="G7" s="47"/>
       <c r="H7" s="47"/>
       <c r="I7" s="48"/>
-      <c r="J7" s="54"/>
-      <c r="K7" s="54"/>
-      <c r="L7" s="50"/>
-      <c r="M7" s="50"/>
-      <c r="N7" s="55">
+      <c r="J7" s="53"/>
+      <c r="K7" s="53"/>
+      <c r="L7" s="49"/>
+      <c r="M7" s="49"/>
+      <c r="N7" s="77">
         <v>3</v>
       </c>
-      <c r="O7" s="55">
+      <c r="O7" s="77">
         <v>0.5</v>
       </c>
-      <c r="P7" s="51"/>
-      <c r="Q7" s="52"/>
-      <c r="R7" s="53"/>
-      <c r="S7" s="51"/>
+      <c r="P7" s="81"/>
+      <c r="Q7" s="51"/>
+      <c r="R7" s="52"/>
+      <c r="S7" s="50"/>
       <c r="T7" s="47"/>
-      <c r="U7" s="51"/>
-      <c r="V7" s="51"/>
-      <c r="W7" s="52"/>
-      <c r="X7" s="53"/>
-      <c r="Y7" s="51"/>
+      <c r="U7" s="50"/>
+      <c r="V7" s="91"/>
+      <c r="W7" s="51"/>
+      <c r="X7" s="52"/>
+      <c r="Y7" s="50"/>
       <c r="Z7" s="47"/>
-      <c r="AA7" s="51"/>
-      <c r="AB7" s="52"/>
-      <c r="AC7" s="53"/>
-      <c r="AD7" s="51"/>
-      <c r="AE7" s="69"/>
-      <c r="AF7" s="72"/>
+      <c r="AA7" s="50"/>
+      <c r="AB7" s="51"/>
+      <c r="AC7" s="52"/>
+      <c r="AD7" s="50"/>
+      <c r="AE7" s="68"/>
+      <c r="AF7" s="70"/>
       <c r="AG7" s="27"/>
       <c r="AH7" s="27"/>
       <c r="AI7" s="27"/>
@@ -2478,7 +2533,7 @@
       </c>
       <c r="D8" s="47">
         <f>IF(SUM(K8:AF8)=0," ",SUM(K8:AF8))</f>
-        <v>1.75</v>
+        <v>2.25</v>
       </c>
       <c r="E8" s="47">
         <v>1</v>
@@ -2487,35 +2542,37 @@
       <c r="G8" s="47"/>
       <c r="H8" s="47"/>
       <c r="I8" s="48"/>
-      <c r="J8" s="54"/>
-      <c r="K8" s="54"/>
-      <c r="L8" s="50"/>
-      <c r="M8" s="50"/>
-      <c r="N8" s="51"/>
-      <c r="O8" s="51"/>
-      <c r="P8" s="55">
+      <c r="J8" s="53"/>
+      <c r="K8" s="53"/>
+      <c r="L8" s="49"/>
+      <c r="M8" s="49"/>
+      <c r="N8" s="81"/>
+      <c r="O8" s="81"/>
+      <c r="P8" s="77">
         <v>0.5</v>
       </c>
-      <c r="Q8" s="52"/>
-      <c r="R8" s="53"/>
-      <c r="S8" s="51"/>
+      <c r="Q8" s="51"/>
+      <c r="R8" s="52"/>
+      <c r="S8" s="50"/>
       <c r="T8" s="47"/>
-      <c r="U8" s="55">
+      <c r="U8" s="77">
         <v>0.75</v>
       </c>
-      <c r="V8" s="56"/>
-      <c r="W8" s="52"/>
-      <c r="X8" s="53"/>
-      <c r="Y8" s="51"/>
+      <c r="V8" s="91"/>
+      <c r="W8" s="51"/>
+      <c r="X8" s="52"/>
+      <c r="Y8" s="50"/>
       <c r="Z8" s="47"/>
-      <c r="AA8" s="55">
+      <c r="AA8" s="77">
         <v>0.5</v>
       </c>
-      <c r="AB8" s="52"/>
-      <c r="AC8" s="53"/>
-      <c r="AD8" s="51"/>
-      <c r="AE8" s="70"/>
-      <c r="AF8" s="72"/>
+      <c r="AB8" s="51"/>
+      <c r="AC8" s="52"/>
+      <c r="AD8" s="50"/>
+      <c r="AE8" s="87">
+        <v>0.5</v>
+      </c>
+      <c r="AF8" s="70"/>
       <c r="AG8" s="27"/>
       <c r="AH8" s="27"/>
       <c r="AI8" s="27"/>
@@ -2548,31 +2605,31 @@
       <c r="G9" s="47"/>
       <c r="H9" s="47"/>
       <c r="I9" s="48"/>
-      <c r="J9" s="54"/>
-      <c r="K9" s="54"/>
-      <c r="L9" s="50"/>
-      <c r="M9" s="50"/>
-      <c r="N9" s="51"/>
-      <c r="O9" s="51"/>
-      <c r="P9" s="55">
+      <c r="J9" s="53"/>
+      <c r="K9" s="53"/>
+      <c r="L9" s="49"/>
+      <c r="M9" s="49"/>
+      <c r="N9" s="81"/>
+      <c r="O9" s="81"/>
+      <c r="P9" s="77">
         <v>1.5</v>
       </c>
-      <c r="Q9" s="52"/>
-      <c r="R9" s="53"/>
-      <c r="S9" s="51"/>
+      <c r="Q9" s="51"/>
+      <c r="R9" s="52"/>
+      <c r="S9" s="50"/>
       <c r="T9" s="47"/>
-      <c r="U9" s="51"/>
-      <c r="V9" s="51"/>
-      <c r="W9" s="52"/>
-      <c r="X9" s="53"/>
-      <c r="Y9" s="51"/>
+      <c r="U9" s="50"/>
+      <c r="V9" s="91"/>
+      <c r="W9" s="51"/>
+      <c r="X9" s="52"/>
+      <c r="Y9" s="50"/>
       <c r="Z9" s="47"/>
-      <c r="AA9" s="51"/>
-      <c r="AB9" s="52"/>
-      <c r="AC9" s="53"/>
-      <c r="AD9" s="51"/>
-      <c r="AE9" s="69"/>
-      <c r="AF9" s="72"/>
+      <c r="AA9" s="50"/>
+      <c r="AB9" s="51"/>
+      <c r="AC9" s="52"/>
+      <c r="AD9" s="50"/>
+      <c r="AE9" s="68"/>
+      <c r="AF9" s="70"/>
       <c r="AG9" s="27"/>
       <c r="AH9" s="27"/>
       <c r="AI9" s="27"/>
@@ -2596,7 +2653,7 @@
       </c>
       <c r="D10" s="47">
         <f>IF(SUM(K10:AF10)=0," ",SUM(K10:AF10))</f>
-        <v>9.5</v>
+        <v>11.5</v>
       </c>
       <c r="E10" s="47">
         <v>1</v>
@@ -2605,39 +2662,41 @@
       <c r="G10" s="47"/>
       <c r="H10" s="47"/>
       <c r="I10" s="48"/>
-      <c r="J10" s="54"/>
-      <c r="K10" s="54"/>
-      <c r="L10" s="50"/>
-      <c r="M10" s="50"/>
-      <c r="N10" s="51"/>
-      <c r="O10" s="56"/>
-      <c r="P10" s="56"/>
-      <c r="Q10" s="52"/>
-      <c r="R10" s="53"/>
-      <c r="S10" s="56">
+      <c r="J10" s="53"/>
+      <c r="K10" s="53"/>
+      <c r="L10" s="49"/>
+      <c r="M10" s="49"/>
+      <c r="N10" s="50"/>
+      <c r="O10" s="55"/>
+      <c r="P10" s="55"/>
+      <c r="Q10" s="51"/>
+      <c r="R10" s="52"/>
+      <c r="S10" s="79">
         <v>2</v>
       </c>
-      <c r="T10" s="57">
+      <c r="T10" s="78">
         <v>3</v>
       </c>
-      <c r="U10" s="56"/>
-      <c r="V10" s="56"/>
-      <c r="W10" s="52"/>
-      <c r="X10" s="53"/>
-      <c r="Y10" s="56"/>
-      <c r="Z10" s="57">
+      <c r="U10" s="55"/>
+      <c r="V10" s="91"/>
+      <c r="W10" s="51"/>
+      <c r="X10" s="52"/>
+      <c r="Y10" s="55"/>
+      <c r="Z10" s="78">
         <v>1.5</v>
       </c>
-      <c r="AA10" s="55">
+      <c r="AA10" s="77">
         <v>1.5</v>
       </c>
-      <c r="AB10" s="52"/>
-      <c r="AC10" s="53"/>
-      <c r="AD10" s="55">
+      <c r="AB10" s="51"/>
+      <c r="AC10" s="52"/>
+      <c r="AD10" s="77">
         <v>1.5</v>
       </c>
-      <c r="AE10" s="70"/>
-      <c r="AF10" s="72"/>
+      <c r="AE10" s="87">
+        <v>2</v>
+      </c>
+      <c r="AF10" s="70"/>
       <c r="AG10" s="27"/>
       <c r="AH10" s="27"/>
       <c r="AI10" s="27"/>
@@ -2668,7 +2727,7 @@
       <c r="F11" s="25"/>
       <c r="G11" s="25"/>
       <c r="H11" s="25"/>
-      <c r="I11" s="58"/>
+      <c r="I11" s="57"/>
       <c r="J11" s="25"/>
       <c r="K11" s="25"/>
       <c r="L11" s="25"/>
@@ -2691,7 +2750,7 @@
       <c r="AC11" s="25"/>
       <c r="AD11" s="25"/>
       <c r="AE11" s="26"/>
-      <c r="AF11" s="72"/>
+      <c r="AF11" s="70"/>
     </row>
     <row r="12" spans="1:42" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="36">
@@ -2714,31 +2773,31 @@
       <c r="G12" s="47"/>
       <c r="H12" s="47"/>
       <c r="I12" s="48"/>
-      <c r="J12" s="54"/>
-      <c r="K12" s="54"/>
-      <c r="L12" s="53"/>
-      <c r="M12" s="52"/>
-      <c r="N12" s="55">
+      <c r="J12" s="53"/>
+      <c r="K12" s="53"/>
+      <c r="L12" s="52"/>
+      <c r="M12" s="51"/>
+      <c r="N12" s="77">
         <v>3</v>
       </c>
-      <c r="O12" s="56"/>
-      <c r="P12" s="51"/>
-      <c r="Q12" s="52"/>
-      <c r="R12" s="53"/>
-      <c r="S12" s="51"/>
+      <c r="O12" s="55"/>
+      <c r="P12" s="50"/>
+      <c r="Q12" s="51"/>
+      <c r="R12" s="52"/>
+      <c r="S12" s="50"/>
       <c r="T12" s="47"/>
       <c r="U12" s="47"/>
-      <c r="V12" s="47"/>
-      <c r="W12" s="52"/>
-      <c r="X12" s="53"/>
-      <c r="Y12" s="51"/>
+      <c r="V12" s="92"/>
+      <c r="W12" s="51"/>
+      <c r="X12" s="52"/>
+      <c r="Y12" s="50"/>
       <c r="Z12" s="47"/>
       <c r="AA12" s="47"/>
-      <c r="AB12" s="52"/>
-      <c r="AC12" s="53"/>
-      <c r="AD12" s="51"/>
-      <c r="AE12" s="69"/>
-      <c r="AF12" s="72"/>
+      <c r="AB12" s="51"/>
+      <c r="AC12" s="52"/>
+      <c r="AD12" s="50"/>
+      <c r="AE12" s="68"/>
+      <c r="AF12" s="70"/>
       <c r="AG12" s="27"/>
       <c r="AH12" s="27"/>
       <c r="AI12" s="27"/>
@@ -2769,31 +2828,31 @@
       <c r="G13" s="47"/>
       <c r="H13" s="47"/>
       <c r="I13" s="48"/>
-      <c r="J13" s="54"/>
-      <c r="K13" s="54"/>
-      <c r="L13" s="53"/>
-      <c r="M13" s="52"/>
-      <c r="N13" s="55">
+      <c r="J13" s="53"/>
+      <c r="K13" s="53"/>
+      <c r="L13" s="52"/>
+      <c r="M13" s="51"/>
+      <c r="N13" s="77">
         <v>1</v>
       </c>
-      <c r="O13" s="51"/>
-      <c r="P13" s="51"/>
-      <c r="Q13" s="52"/>
-      <c r="R13" s="53"/>
-      <c r="S13" s="51"/>
+      <c r="O13" s="50"/>
+      <c r="P13" s="50"/>
+      <c r="Q13" s="51"/>
+      <c r="R13" s="52"/>
+      <c r="S13" s="50"/>
       <c r="T13" s="47"/>
       <c r="U13" s="47"/>
-      <c r="V13" s="47"/>
-      <c r="W13" s="52"/>
-      <c r="X13" s="53"/>
-      <c r="Y13" s="51"/>
+      <c r="V13" s="92"/>
+      <c r="W13" s="51"/>
+      <c r="X13" s="52"/>
+      <c r="Y13" s="50"/>
       <c r="Z13" s="47"/>
       <c r="AA13" s="47"/>
-      <c r="AB13" s="52"/>
-      <c r="AC13" s="53"/>
-      <c r="AD13" s="51"/>
-      <c r="AE13" s="69"/>
-      <c r="AF13" s="72"/>
+      <c r="AB13" s="51"/>
+      <c r="AC13" s="52"/>
+      <c r="AD13" s="50"/>
+      <c r="AE13" s="68"/>
+      <c r="AF13" s="70"/>
       <c r="AG13" s="27"/>
       <c r="AH13" s="27"/>
       <c r="AI13" s="27"/>
@@ -2820,29 +2879,29 @@
       <c r="G14" s="47"/>
       <c r="H14" s="47"/>
       <c r="I14" s="48"/>
-      <c r="J14" s="54"/>
-      <c r="K14" s="54"/>
-      <c r="L14" s="53"/>
-      <c r="M14" s="52"/>
-      <c r="N14" s="51"/>
-      <c r="O14" s="51"/>
-      <c r="P14" s="51"/>
-      <c r="Q14" s="52"/>
-      <c r="R14" s="53"/>
-      <c r="S14" s="51"/>
+      <c r="J14" s="53"/>
+      <c r="K14" s="53"/>
+      <c r="L14" s="52"/>
+      <c r="M14" s="51"/>
+      <c r="N14" s="50"/>
+      <c r="O14" s="50"/>
+      <c r="P14" s="50"/>
+      <c r="Q14" s="51"/>
+      <c r="R14" s="52"/>
+      <c r="S14" s="50"/>
       <c r="T14" s="47"/>
       <c r="U14" s="47"/>
-      <c r="V14" s="47"/>
-      <c r="W14" s="52"/>
-      <c r="X14" s="53"/>
-      <c r="Y14" s="51"/>
+      <c r="V14" s="92"/>
+      <c r="W14" s="51"/>
+      <c r="X14" s="52"/>
+      <c r="Y14" s="50"/>
       <c r="Z14" s="47"/>
       <c r="AA14" s="47"/>
-      <c r="AB14" s="52"/>
-      <c r="AC14" s="53"/>
-      <c r="AD14" s="51"/>
-      <c r="AE14" s="69"/>
-      <c r="AF14" s="72"/>
+      <c r="AB14" s="51"/>
+      <c r="AC14" s="52"/>
+      <c r="AD14" s="50"/>
+      <c r="AE14" s="68"/>
+      <c r="AF14" s="70"/>
       <c r="AG14" s="27"/>
       <c r="AH14" s="27"/>
       <c r="AI14" s="27"/>
@@ -2869,29 +2928,29 @@
       <c r="G15" s="47"/>
       <c r="H15" s="47"/>
       <c r="I15" s="48"/>
-      <c r="J15" s="54"/>
-      <c r="K15" s="54"/>
-      <c r="L15" s="53"/>
-      <c r="M15" s="52"/>
-      <c r="N15" s="51"/>
-      <c r="O15" s="51"/>
-      <c r="P15" s="51"/>
-      <c r="Q15" s="52"/>
-      <c r="R15" s="53"/>
-      <c r="S15" s="51"/>
+      <c r="J15" s="53"/>
+      <c r="K15" s="53"/>
+      <c r="L15" s="52"/>
+      <c r="M15" s="51"/>
+      <c r="N15" s="50"/>
+      <c r="O15" s="50"/>
+      <c r="P15" s="50"/>
+      <c r="Q15" s="51"/>
+      <c r="R15" s="52"/>
+      <c r="S15" s="50"/>
       <c r="T15" s="47"/>
       <c r="U15" s="47"/>
-      <c r="V15" s="47"/>
-      <c r="W15" s="52"/>
-      <c r="X15" s="53"/>
-      <c r="Y15" s="51"/>
+      <c r="V15" s="92"/>
+      <c r="W15" s="51"/>
+      <c r="X15" s="52"/>
+      <c r="Y15" s="50"/>
       <c r="Z15" s="47"/>
       <c r="AA15" s="47"/>
-      <c r="AB15" s="52"/>
-      <c r="AC15" s="53"/>
-      <c r="AD15" s="51"/>
-      <c r="AE15" s="69"/>
-      <c r="AF15" s="72"/>
+      <c r="AB15" s="51"/>
+      <c r="AC15" s="52"/>
+      <c r="AD15" s="50"/>
+      <c r="AE15" s="68"/>
+      <c r="AF15" s="70"/>
       <c r="AG15" s="27"/>
       <c r="AH15" s="27"/>
       <c r="AI15" s="27"/>
@@ -2916,13 +2975,13 @@
       </c>
       <c r="D16" s="45">
         <f>SUM(D17:D24)</f>
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E16" s="15"/>
       <c r="F16" s="25"/>
       <c r="G16" s="25"/>
       <c r="H16" s="25"/>
-      <c r="I16" s="58"/>
+      <c r="I16" s="57"/>
       <c r="J16" s="25"/>
       <c r="K16" s="30"/>
       <c r="L16" s="30"/>
@@ -2945,13 +3004,13 @@
       <c r="AC16" s="25"/>
       <c r="AD16" s="25"/>
       <c r="AE16" s="26"/>
-      <c r="AF16" s="72"/>
+      <c r="AF16" s="70"/>
     </row>
     <row r="17" spans="1:42" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="36">
         <v>31</v>
       </c>
-      <c r="B17" s="59" t="s">
+      <c r="B17" s="58" t="s">
         <v>48</v>
       </c>
       <c r="C17" s="47">
@@ -2968,33 +3027,33 @@
       <c r="G17" s="47"/>
       <c r="H17" s="47"/>
       <c r="I17" s="48"/>
-      <c r="J17" s="54"/>
-      <c r="K17" s="54"/>
-      <c r="L17" s="53"/>
-      <c r="M17" s="52"/>
-      <c r="N17" s="55">
+      <c r="J17" s="53"/>
+      <c r="K17" s="53"/>
+      <c r="L17" s="52"/>
+      <c r="M17" s="51"/>
+      <c r="N17" s="77">
         <v>0.8</v>
       </c>
-      <c r="O17" s="55">
+      <c r="O17" s="77">
         <v>0.5</v>
       </c>
-      <c r="P17" s="51"/>
-      <c r="Q17" s="52"/>
-      <c r="R17" s="53"/>
-      <c r="S17" s="51"/>
+      <c r="P17" s="81"/>
+      <c r="Q17" s="51"/>
+      <c r="R17" s="52"/>
+      <c r="S17" s="50"/>
       <c r="T17" s="47"/>
-      <c r="U17" s="51"/>
-      <c r="V17" s="51"/>
-      <c r="W17" s="52"/>
-      <c r="X17" s="53"/>
-      <c r="Y17" s="51"/>
+      <c r="U17" s="50"/>
+      <c r="V17" s="91"/>
+      <c r="W17" s="51"/>
+      <c r="X17" s="52"/>
+      <c r="Y17" s="50"/>
       <c r="Z17" s="47"/>
-      <c r="AA17" s="51"/>
-      <c r="AB17" s="52"/>
-      <c r="AC17" s="53"/>
-      <c r="AD17" s="51"/>
-      <c r="AE17" s="69"/>
-      <c r="AF17" s="72"/>
+      <c r="AA17" s="50"/>
+      <c r="AB17" s="51"/>
+      <c r="AC17" s="52"/>
+      <c r="AD17" s="50"/>
+      <c r="AE17" s="68"/>
+      <c r="AF17" s="70"/>
       <c r="AG17" s="27"/>
       <c r="AH17" s="27"/>
       <c r="AI17" s="27"/>
@@ -3010,7 +3069,7 @@
       <c r="A18" s="36">
         <v>32</v>
       </c>
-      <c r="B18" s="59" t="s">
+      <c r="B18" s="58" t="s">
         <v>39</v>
       </c>
       <c r="C18" s="47">
@@ -3027,31 +3086,31 @@
       <c r="G18" s="47"/>
       <c r="H18" s="47"/>
       <c r="I18" s="48"/>
-      <c r="J18" s="54"/>
-      <c r="K18" s="54"/>
-      <c r="L18" s="53"/>
-      <c r="M18" s="52"/>
-      <c r="N18" s="51"/>
-      <c r="O18" s="78">
+      <c r="J18" s="53"/>
+      <c r="K18" s="53"/>
+      <c r="L18" s="52"/>
+      <c r="M18" s="51"/>
+      <c r="N18" s="81"/>
+      <c r="O18" s="85">
         <v>3</v>
       </c>
-      <c r="P18" s="61"/>
-      <c r="Q18" s="52"/>
-      <c r="R18" s="53"/>
-      <c r="S18" s="56"/>
+      <c r="P18" s="86"/>
+      <c r="Q18" s="51"/>
+      <c r="R18" s="52"/>
+      <c r="S18" s="55"/>
       <c r="T18" s="47"/>
-      <c r="U18" s="51"/>
-      <c r="V18" s="51"/>
-      <c r="W18" s="52"/>
-      <c r="X18" s="53"/>
-      <c r="Y18" s="51"/>
+      <c r="U18" s="50"/>
+      <c r="V18" s="91"/>
+      <c r="W18" s="51"/>
+      <c r="X18" s="52"/>
+      <c r="Y18" s="50"/>
       <c r="Z18" s="47"/>
-      <c r="AA18" s="51"/>
-      <c r="AB18" s="52"/>
-      <c r="AC18" s="53"/>
-      <c r="AD18" s="51"/>
-      <c r="AE18" s="69"/>
-      <c r="AF18" s="72"/>
+      <c r="AA18" s="50"/>
+      <c r="AB18" s="51"/>
+      <c r="AC18" s="52"/>
+      <c r="AD18" s="50"/>
+      <c r="AE18" s="68"/>
+      <c r="AF18" s="70"/>
       <c r="AG18" s="27"/>
       <c r="AH18" s="27"/>
       <c r="AI18" s="27"/>
@@ -3067,7 +3126,7 @@
       <c r="A19" s="36">
         <v>33</v>
       </c>
-      <c r="B19" s="59" t="s">
+      <c r="B19" s="58" t="s">
         <v>40</v>
       </c>
       <c r="C19" s="47">
@@ -3084,33 +3143,33 @@
       <c r="G19" s="47"/>
       <c r="H19" s="47"/>
       <c r="I19" s="48"/>
-      <c r="J19" s="54"/>
-      <c r="K19" s="54"/>
-      <c r="L19" s="53"/>
-      <c r="M19" s="52"/>
-      <c r="N19" s="51"/>
-      <c r="O19" s="51">
+      <c r="J19" s="53"/>
+      <c r="K19" s="53"/>
+      <c r="L19" s="52"/>
+      <c r="M19" s="51"/>
+      <c r="N19" s="81"/>
+      <c r="O19" s="81">
         <v>1</v>
       </c>
-      <c r="P19" s="55">
+      <c r="P19" s="77">
         <v>3</v>
       </c>
-      <c r="Q19" s="52"/>
-      <c r="R19" s="53"/>
-      <c r="S19" s="51"/>
-      <c r="T19" s="57"/>
-      <c r="U19" s="56"/>
-      <c r="V19" s="56"/>
-      <c r="W19" s="52"/>
-      <c r="X19" s="53"/>
-      <c r="Y19" s="56"/>
-      <c r="Z19" s="57"/>
-      <c r="AA19" s="56"/>
-      <c r="AB19" s="52"/>
-      <c r="AC19" s="53"/>
-      <c r="AD19" s="51"/>
-      <c r="AE19" s="69"/>
-      <c r="AF19" s="72"/>
+      <c r="Q19" s="51"/>
+      <c r="R19" s="52"/>
+      <c r="S19" s="50"/>
+      <c r="T19" s="56"/>
+      <c r="U19" s="55"/>
+      <c r="V19" s="91"/>
+      <c r="W19" s="51"/>
+      <c r="X19" s="52"/>
+      <c r="Y19" s="55"/>
+      <c r="Z19" s="56"/>
+      <c r="AA19" s="55"/>
+      <c r="AB19" s="51"/>
+      <c r="AC19" s="52"/>
+      <c r="AD19" s="50"/>
+      <c r="AE19" s="68"/>
+      <c r="AF19" s="70"/>
       <c r="AG19" s="27"/>
       <c r="AH19" s="27"/>
       <c r="AI19" s="27"/>
@@ -3126,7 +3185,7 @@
       <c r="A20" s="36">
         <v>34</v>
       </c>
-      <c r="B20" s="59" t="s">
+      <c r="B20" s="58" t="s">
         <v>41</v>
       </c>
       <c r="C20" s="47">
@@ -3143,37 +3202,37 @@
       <c r="G20" s="47"/>
       <c r="H20" s="47"/>
       <c r="I20" s="48"/>
-      <c r="J20" s="54"/>
-      <c r="K20" s="54"/>
-      <c r="L20" s="53"/>
-      <c r="M20" s="52"/>
-      <c r="N20" s="51"/>
-      <c r="O20" s="51">
+      <c r="J20" s="53"/>
+      <c r="K20" s="53"/>
+      <c r="L20" s="52"/>
+      <c r="M20" s="51"/>
+      <c r="N20" s="81"/>
+      <c r="O20" s="81">
         <v>2.5</v>
       </c>
-      <c r="P20" s="55">
+      <c r="P20" s="77">
         <v>1.5</v>
       </c>
-      <c r="Q20" s="52"/>
-      <c r="R20" s="53"/>
-      <c r="S20" s="55">
+      <c r="Q20" s="51"/>
+      <c r="R20" s="52"/>
+      <c r="S20" s="77">
         <v>1.5</v>
       </c>
       <c r="T20" s="47"/>
-      <c r="U20" s="56"/>
-      <c r="V20" s="56"/>
-      <c r="W20" s="52"/>
-      <c r="X20" s="53"/>
-      <c r="Y20" s="56"/>
-      <c r="Z20" s="57">
+      <c r="U20" s="55"/>
+      <c r="V20" s="91"/>
+      <c r="W20" s="51"/>
+      <c r="X20" s="52"/>
+      <c r="Y20" s="55"/>
+      <c r="Z20" s="78">
         <v>0.5</v>
       </c>
-      <c r="AA20" s="56"/>
-      <c r="AB20" s="52"/>
-      <c r="AC20" s="53"/>
-      <c r="AD20" s="51"/>
-      <c r="AE20" s="69"/>
-      <c r="AF20" s="72"/>
+      <c r="AA20" s="55"/>
+      <c r="AB20" s="51"/>
+      <c r="AC20" s="52"/>
+      <c r="AD20" s="50"/>
+      <c r="AE20" s="68"/>
+      <c r="AF20" s="70"/>
       <c r="AG20" s="27"/>
       <c r="AH20" s="27"/>
       <c r="AI20" s="27"/>
@@ -3189,7 +3248,7 @@
       <c r="A21" s="36">
         <v>35</v>
       </c>
-      <c r="B21" s="59" t="s">
+      <c r="B21" s="58" t="s">
         <v>42</v>
       </c>
       <c r="C21" s="47">
@@ -3206,37 +3265,37 @@
       <c r="G21" s="47"/>
       <c r="H21" s="47"/>
       <c r="I21" s="48"/>
-      <c r="J21" s="54"/>
-      <c r="K21" s="54"/>
-      <c r="L21" s="53"/>
-      <c r="M21" s="52"/>
-      <c r="N21" s="51"/>
-      <c r="O21" s="51"/>
-      <c r="P21" s="51"/>
-      <c r="Q21" s="52"/>
-      <c r="R21" s="53"/>
-      <c r="S21" s="55">
+      <c r="J21" s="53"/>
+      <c r="K21" s="53"/>
+      <c r="L21" s="52"/>
+      <c r="M21" s="51"/>
+      <c r="N21" s="50"/>
+      <c r="O21" s="50"/>
+      <c r="P21" s="50"/>
+      <c r="Q21" s="51"/>
+      <c r="R21" s="52"/>
+      <c r="S21" s="77">
         <v>0.5</v>
       </c>
-      <c r="T21" s="49">
+      <c r="T21" s="82">
         <v>1.2</v>
       </c>
-      <c r="U21" s="51">
+      <c r="U21" s="81">
         <v>0.5</v>
       </c>
-      <c r="V21" s="51"/>
-      <c r="W21" s="52"/>
-      <c r="X21" s="53"/>
-      <c r="Y21" s="56"/>
-      <c r="Z21" s="57">
+      <c r="V21" s="91"/>
+      <c r="W21" s="51"/>
+      <c r="X21" s="52"/>
+      <c r="Y21" s="55"/>
+      <c r="Z21" s="78">
         <v>0.5</v>
       </c>
-      <c r="AA21" s="56"/>
-      <c r="AB21" s="52"/>
-      <c r="AC21" s="53"/>
-      <c r="AD21" s="51"/>
-      <c r="AE21" s="69"/>
-      <c r="AF21" s="72"/>
+      <c r="AA21" s="55"/>
+      <c r="AB21" s="51"/>
+      <c r="AC21" s="52"/>
+      <c r="AD21" s="50"/>
+      <c r="AE21" s="68"/>
+      <c r="AF21" s="70"/>
       <c r="AG21" s="27"/>
       <c r="AH21" s="27"/>
       <c r="AI21" s="27"/>
@@ -3252,7 +3311,7 @@
       <c r="A22" s="36">
         <v>36</v>
       </c>
-      <c r="B22" s="59" t="s">
+      <c r="B22" s="58" t="s">
         <v>43</v>
       </c>
       <c r="C22" s="47">
@@ -3260,7 +3319,7 @@
       </c>
       <c r="D22" s="47">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E22" s="47">
         <v>1</v>
@@ -3269,37 +3328,39 @@
       <c r="G22" s="47"/>
       <c r="H22" s="47"/>
       <c r="I22" s="48"/>
-      <c r="J22" s="54"/>
-      <c r="K22" s="54"/>
-      <c r="L22" s="53"/>
-      <c r="M22" s="52"/>
-      <c r="N22" s="51"/>
-      <c r="O22" s="51"/>
-      <c r="P22" s="51"/>
-      <c r="Q22" s="52"/>
-      <c r="R22" s="53"/>
-      <c r="S22" s="51">
+      <c r="J22" s="53"/>
+      <c r="K22" s="53"/>
+      <c r="L22" s="52"/>
+      <c r="M22" s="51"/>
+      <c r="N22" s="50"/>
+      <c r="O22" s="50"/>
+      <c r="P22" s="50"/>
+      <c r="Q22" s="51"/>
+      <c r="R22" s="52"/>
+      <c r="S22" s="81">
         <v>2.5</v>
       </c>
-      <c r="T22" s="49">
+      <c r="T22" s="82">
         <v>2</v>
       </c>
-      <c r="U22" s="51">
+      <c r="U22" s="81">
         <v>2</v>
       </c>
-      <c r="V22" s="51"/>
-      <c r="W22" s="52"/>
-      <c r="X22" s="53"/>
-      <c r="Y22" s="56"/>
-      <c r="Z22" s="57">
+      <c r="V22" s="91"/>
+      <c r="W22" s="51"/>
+      <c r="X22" s="52"/>
+      <c r="Y22" s="55"/>
+      <c r="Z22" s="78">
         <v>1.5</v>
       </c>
-      <c r="AA22" s="56"/>
-      <c r="AB22" s="52"/>
-      <c r="AC22" s="53"/>
-      <c r="AD22" s="51"/>
-      <c r="AE22" s="69"/>
-      <c r="AF22" s="72"/>
+      <c r="AA22" s="55"/>
+      <c r="AB22" s="51"/>
+      <c r="AC22" s="52"/>
+      <c r="AD22" s="81">
+        <v>1</v>
+      </c>
+      <c r="AE22" s="68"/>
+      <c r="AF22" s="70"/>
       <c r="AG22" s="27"/>
       <c r="AH22" s="27"/>
       <c r="AI22" s="27"/>
@@ -3312,8 +3373,8 @@
       <c r="AP22" s="27"/>
     </row>
     <row r="23" spans="1:42" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="80"/>
-      <c r="B23" s="59" t="s">
+      <c r="A23" s="76"/>
+      <c r="B23" s="58" t="s">
         <v>54</v>
       </c>
       <c r="C23" s="47">
@@ -3321,40 +3382,42 @@
       </c>
       <c r="D23" s="47">
         <f t="shared" si="0"/>
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
       <c r="E23" s="47"/>
       <c r="F23" s="47"/>
       <c r="G23" s="47"/>
       <c r="H23" s="47"/>
       <c r="I23" s="48"/>
-      <c r="J23" s="54"/>
-      <c r="K23" s="54"/>
-      <c r="L23" s="53"/>
-      <c r="M23" s="52"/>
-      <c r="N23" s="51"/>
-      <c r="O23" s="51"/>
-      <c r="P23" s="51"/>
-      <c r="Q23" s="52"/>
-      <c r="R23" s="53"/>
-      <c r="S23" s="51"/>
-      <c r="T23" s="57"/>
-      <c r="U23" s="51"/>
-      <c r="V23" s="51"/>
-      <c r="W23" s="52"/>
-      <c r="X23" s="53"/>
-      <c r="Y23" s="56"/>
-      <c r="Z23" s="57"/>
-      <c r="AA23" s="55">
+      <c r="J23" s="53"/>
+      <c r="K23" s="53"/>
+      <c r="L23" s="52"/>
+      <c r="M23" s="51"/>
+      <c r="N23" s="50"/>
+      <c r="O23" s="50"/>
+      <c r="P23" s="50"/>
+      <c r="Q23" s="51"/>
+      <c r="R23" s="52"/>
+      <c r="S23" s="50"/>
+      <c r="T23" s="56"/>
+      <c r="U23" s="50"/>
+      <c r="V23" s="91"/>
+      <c r="W23" s="51"/>
+      <c r="X23" s="52"/>
+      <c r="Y23" s="55"/>
+      <c r="Z23" s="56"/>
+      <c r="AA23" s="77">
         <v>0.5</v>
       </c>
-      <c r="AB23" s="52"/>
-      <c r="AC23" s="53"/>
-      <c r="AD23" s="55">
+      <c r="AB23" s="51"/>
+      <c r="AC23" s="52"/>
+      <c r="AD23" s="77">
         <v>2</v>
       </c>
-      <c r="AE23" s="69"/>
-      <c r="AF23" s="72"/>
+      <c r="AE23" s="68">
+        <v>1</v>
+      </c>
+      <c r="AF23" s="70"/>
       <c r="AG23" s="27"/>
       <c r="AH23" s="27"/>
       <c r="AI23" s="27"/>
@@ -3370,7 +3433,7 @@
       <c r="A24" s="36">
         <v>37</v>
       </c>
-      <c r="B24" s="59" t="s">
+      <c r="B24" s="58" t="s">
         <v>44</v>
       </c>
       <c r="C24" s="47">
@@ -3387,37 +3450,37 @@
       <c r="G24" s="47"/>
       <c r="H24" s="47"/>
       <c r="I24" s="48"/>
-      <c r="J24" s="54"/>
-      <c r="K24" s="54"/>
-      <c r="L24" s="53"/>
-      <c r="M24" s="52" t="s">
+      <c r="J24" s="53"/>
+      <c r="K24" s="53"/>
+      <c r="L24" s="52"/>
+      <c r="M24" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="N24" s="51"/>
-      <c r="O24" s="51"/>
-      <c r="P24" s="51"/>
-      <c r="Q24" s="52"/>
-      <c r="R24" s="53"/>
-      <c r="S24" s="51">
+      <c r="N24" s="50"/>
+      <c r="O24" s="50"/>
+      <c r="P24" s="50"/>
+      <c r="Q24" s="51"/>
+      <c r="R24" s="52"/>
+      <c r="S24" s="81">
         <v>0.5</v>
       </c>
-      <c r="T24" s="47">
+      <c r="T24" s="83">
         <v>0.5</v>
       </c>
-      <c r="U24" s="55"/>
-      <c r="V24" s="55"/>
-      <c r="W24" s="52"/>
-      <c r="X24" s="53"/>
-      <c r="Y24" s="56">
+      <c r="U24" s="54"/>
+      <c r="V24" s="91"/>
+      <c r="W24" s="51"/>
+      <c r="X24" s="52"/>
+      <c r="Y24" s="79">
         <v>0.5</v>
       </c>
-      <c r="Z24" s="57"/>
-      <c r="AA24" s="56"/>
-      <c r="AB24" s="52"/>
-      <c r="AC24" s="53"/>
-      <c r="AD24" s="51"/>
-      <c r="AE24" s="69"/>
-      <c r="AF24" s="72"/>
+      <c r="Z24" s="78"/>
+      <c r="AA24" s="79"/>
+      <c r="AB24" s="51"/>
+      <c r="AC24" s="52"/>
+      <c r="AD24" s="50"/>
+      <c r="AE24" s="68"/>
+      <c r="AF24" s="70"/>
       <c r="AG24" s="27"/>
       <c r="AH24" s="27"/>
       <c r="AI24" s="27"/>
@@ -3438,17 +3501,17 @@
       </c>
       <c r="C25" s="25">
         <f>SUM(C26:C27)</f>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D25" s="45">
         <f>SUM(D26:D27)</f>
-        <v>19.5</v>
+        <v>22.5</v>
       </c>
       <c r="E25" s="15"/>
       <c r="F25" s="25"/>
       <c r="G25" s="25"/>
       <c r="H25" s="25"/>
-      <c r="I25" s="58"/>
+      <c r="I25" s="57"/>
       <c r="J25" s="30"/>
       <c r="K25" s="30"/>
       <c r="L25" s="30"/>
@@ -3464,20 +3527,20 @@
       <c r="V25" s="30"/>
       <c r="W25" s="25"/>
       <c r="X25" s="25"/>
-      <c r="Y25" s="25"/>
-      <c r="Z25" s="25"/>
-      <c r="AA25" s="25"/>
+      <c r="Y25" s="80"/>
+      <c r="Z25" s="80"/>
+      <c r="AA25" s="80"/>
       <c r="AB25" s="25"/>
       <c r="AC25" s="25"/>
       <c r="AD25" s="25"/>
       <c r="AE25" s="26"/>
-      <c r="AF25" s="72"/>
+      <c r="AF25" s="70"/>
     </row>
     <row r="26" spans="1:42" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="36">
         <v>41</v>
       </c>
-      <c r="B26" s="59" t="s">
+      <c r="B26" s="58" t="s">
         <v>45</v>
       </c>
       <c r="C26" s="47">
@@ -3485,7 +3548,7 @@
       </c>
       <c r="D26" s="47">
         <f>IF(SUM(K26:AF26)=0," ",SUM(K26:AF26))</f>
-        <v>5.5</v>
+        <v>7</v>
       </c>
       <c r="E26" s="47">
         <v>1</v>
@@ -3494,39 +3557,41 @@
       <c r="G26" s="47"/>
       <c r="H26" s="47"/>
       <c r="I26" s="48"/>
-      <c r="J26" s="60"/>
-      <c r="K26" s="60"/>
-      <c r="L26" s="53"/>
-      <c r="M26" s="52"/>
-      <c r="N26" s="51"/>
-      <c r="O26" s="51"/>
-      <c r="P26" s="51"/>
-      <c r="Q26" s="52"/>
-      <c r="R26" s="53"/>
-      <c r="S26" s="51"/>
-      <c r="T26" s="47">
+      <c r="J26" s="59"/>
+      <c r="K26" s="59"/>
+      <c r="L26" s="52"/>
+      <c r="M26" s="51"/>
+      <c r="N26" s="50"/>
+      <c r="O26" s="50"/>
+      <c r="P26" s="50"/>
+      <c r="Q26" s="51"/>
+      <c r="R26" s="52"/>
+      <c r="S26" s="50"/>
+      <c r="T26" s="83">
         <v>0.5</v>
       </c>
-      <c r="U26" s="55">
+      <c r="U26" s="77">
         <v>1</v>
       </c>
-      <c r="V26" s="55"/>
-      <c r="W26" s="52"/>
-      <c r="X26" s="53"/>
-      <c r="Y26" s="55">
+      <c r="V26" s="91"/>
+      <c r="W26" s="51"/>
+      <c r="X26" s="52"/>
+      <c r="Y26" s="77">
         <v>2.5</v>
       </c>
-      <c r="Z26" s="57">
+      <c r="Z26" s="78">
         <v>0.5</v>
       </c>
-      <c r="AA26" s="56">
+      <c r="AA26" s="79">
         <v>1</v>
       </c>
-      <c r="AB26" s="52"/>
-      <c r="AC26" s="53"/>
-      <c r="AD26" s="51"/>
-      <c r="AE26" s="69"/>
-      <c r="AF26" s="72"/>
+      <c r="AB26" s="51"/>
+      <c r="AC26" s="52"/>
+      <c r="AD26" s="50"/>
+      <c r="AE26" s="68">
+        <v>1.5</v>
+      </c>
+      <c r="AF26" s="70"/>
       <c r="AG26" s="27"/>
       <c r="AH26" s="27"/>
       <c r="AI26" s="27"/>
@@ -3542,15 +3607,15 @@
       <c r="A27" s="36">
         <v>42</v>
       </c>
-      <c r="B27" s="59" t="s">
+      <c r="B27" s="58" t="s">
         <v>12</v>
       </c>
       <c r="C27" s="47">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D27" s="47">
         <f>IF(SUM(K27:AF27)=0," ",SUM(K27:AF27))</f>
-        <v>14</v>
+        <v>15.5</v>
       </c>
       <c r="E27" s="47">
         <v>1</v>
@@ -3559,39 +3624,41 @@
       <c r="G27" s="47"/>
       <c r="H27" s="47"/>
       <c r="I27" s="48"/>
-      <c r="J27" s="60"/>
-      <c r="K27" s="60"/>
-      <c r="L27" s="53"/>
-      <c r="M27" s="52"/>
-      <c r="N27" s="51"/>
-      <c r="O27" s="51"/>
-      <c r="P27" s="51"/>
-      <c r="Q27" s="52"/>
-      <c r="R27" s="53"/>
-      <c r="S27" s="51"/>
-      <c r="T27" s="47"/>
-      <c r="U27" s="51">
+      <c r="J27" s="59"/>
+      <c r="K27" s="59"/>
+      <c r="L27" s="52"/>
+      <c r="M27" s="51"/>
+      <c r="N27" s="50"/>
+      <c r="O27" s="50"/>
+      <c r="P27" s="50"/>
+      <c r="Q27" s="51"/>
+      <c r="R27" s="52"/>
+      <c r="S27" s="50"/>
+      <c r="T27" s="83"/>
+      <c r="U27" s="81">
         <v>3</v>
       </c>
-      <c r="V27" s="51"/>
-      <c r="W27" s="52"/>
-      <c r="X27" s="53"/>
-      <c r="Y27" s="51">
+      <c r="V27" s="91"/>
+      <c r="W27" s="51"/>
+      <c r="X27" s="52"/>
+      <c r="Y27" s="81">
         <v>4</v>
       </c>
-      <c r="Z27" s="49">
+      <c r="Z27" s="82">
         <v>3</v>
       </c>
-      <c r="AA27" s="51">
+      <c r="AA27" s="81">
         <v>2</v>
       </c>
-      <c r="AB27" s="52"/>
-      <c r="AC27" s="53"/>
-      <c r="AD27" s="51">
-        <v>2</v>
-      </c>
-      <c r="AE27" s="69"/>
-      <c r="AF27" s="72"/>
+      <c r="AB27" s="51"/>
+      <c r="AC27" s="52"/>
+      <c r="AD27" s="81">
+        <v>2.5</v>
+      </c>
+      <c r="AE27" s="90">
+        <v>1</v>
+      </c>
+      <c r="AF27" s="70"/>
       <c r="AG27" s="27"/>
       <c r="AH27" s="27"/>
       <c r="AI27" s="27"/>
@@ -3616,42 +3683,42 @@
       </c>
       <c r="D28" s="45">
         <f>SUM(D29:D30)</f>
-        <v>1.5</v>
+        <v>4.5</v>
       </c>
       <c r="E28" s="15"/>
       <c r="F28" s="25"/>
       <c r="G28" s="25"/>
       <c r="H28" s="25"/>
-      <c r="I28" s="58"/>
+      <c r="I28" s="57"/>
       <c r="J28" s="25"/>
       <c r="K28" s="25"/>
-      <c r="L28" s="68"/>
-      <c r="M28" s="68"/>
-      <c r="N28" s="68"/>
-      <c r="O28" s="68"/>
-      <c r="P28" s="68"/>
-      <c r="Q28" s="68"/>
-      <c r="R28" s="68"/>
-      <c r="S28" s="68"/>
-      <c r="T28" s="68"/>
-      <c r="U28" s="68"/>
-      <c r="V28" s="68"/>
+      <c r="L28" s="67"/>
+      <c r="M28" s="67"/>
+      <c r="N28" s="67"/>
+      <c r="O28" s="67"/>
+      <c r="P28" s="67"/>
+      <c r="Q28" s="67"/>
+      <c r="R28" s="67"/>
+      <c r="S28" s="67"/>
+      <c r="T28" s="67"/>
+      <c r="U28" s="67"/>
+      <c r="V28" s="67"/>
       <c r="W28" s="25"/>
       <c r="X28" s="25"/>
-      <c r="Y28" s="25"/>
-      <c r="Z28" s="25"/>
-      <c r="AA28" s="25"/>
+      <c r="Y28" s="80"/>
+      <c r="Z28" s="80"/>
+      <c r="AA28" s="80"/>
       <c r="AB28" s="25"/>
       <c r="AC28" s="25"/>
       <c r="AD28" s="25"/>
       <c r="AE28" s="26"/>
-      <c r="AF28" s="72"/>
+      <c r="AF28" s="70"/>
     </row>
     <row r="29" spans="1:42" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="36">
         <v>51</v>
       </c>
-      <c r="B29" s="59" t="s">
+      <c r="B29" s="58" t="s">
         <v>50</v>
       </c>
       <c r="C29" s="47">
@@ -3668,31 +3735,31 @@
       <c r="G29" s="47"/>
       <c r="H29" s="47"/>
       <c r="I29" s="48"/>
-      <c r="J29" s="60"/>
-      <c r="K29" s="60"/>
-      <c r="L29" s="53"/>
-      <c r="M29" s="52"/>
-      <c r="N29" s="51"/>
-      <c r="O29" s="51"/>
-      <c r="P29" s="51">
+      <c r="J29" s="59"/>
+      <c r="K29" s="59"/>
+      <c r="L29" s="52"/>
+      <c r="M29" s="51"/>
+      <c r="N29" s="50"/>
+      <c r="O29" s="50"/>
+      <c r="P29" s="81">
         <v>0.5</v>
       </c>
-      <c r="Q29" s="52"/>
-      <c r="R29" s="53"/>
-      <c r="S29" s="51"/>
+      <c r="Q29" s="51"/>
+      <c r="R29" s="52"/>
+      <c r="S29" s="50"/>
       <c r="T29" s="47"/>
-      <c r="U29" s="51"/>
-      <c r="V29" s="51"/>
-      <c r="W29" s="52"/>
-      <c r="X29" s="53"/>
-      <c r="Y29" s="51"/>
-      <c r="Z29" s="47"/>
-      <c r="AA29" s="51"/>
-      <c r="AB29" s="52"/>
-      <c r="AC29" s="53"/>
-      <c r="AD29" s="51"/>
-      <c r="AE29" s="69"/>
-      <c r="AF29" s="72"/>
+      <c r="U29" s="50"/>
+      <c r="V29" s="91"/>
+      <c r="W29" s="51"/>
+      <c r="X29" s="52"/>
+      <c r="Y29" s="81"/>
+      <c r="Z29" s="83"/>
+      <c r="AA29" s="81"/>
+      <c r="AB29" s="51"/>
+      <c r="AC29" s="52"/>
+      <c r="AD29" s="50"/>
+      <c r="AE29" s="68"/>
+      <c r="AF29" s="70"/>
       <c r="AG29" s="27"/>
       <c r="AH29" s="27"/>
       <c r="AI29" s="27"/>
@@ -3708,45 +3775,47 @@
       <c r="A30" s="36">
         <v>52</v>
       </c>
-      <c r="B30" s="59" t="s">
+      <c r="B30" s="58" t="s">
         <v>52</v>
       </c>
       <c r="C30" s="47">
         <v>5</v>
       </c>
       <c r="D30" s="47">
-        <v>1</v>
-      </c>
-      <c r="E30" s="47"/>
+        <v>4</v>
+      </c>
+      <c r="E30" s="47">
+        <v>3</v>
+      </c>
       <c r="F30" s="47"/>
       <c r="G30" s="47"/>
       <c r="H30" s="47"/>
       <c r="I30" s="48"/>
-      <c r="J30" s="54"/>
-      <c r="K30" s="54"/>
-      <c r="L30" s="53"/>
-      <c r="M30" s="52"/>
-      <c r="N30" s="51"/>
-      <c r="O30" s="51"/>
-      <c r="P30" s="51"/>
-      <c r="Q30" s="52"/>
-      <c r="R30" s="53"/>
-      <c r="S30" s="51"/>
+      <c r="J30" s="53"/>
+      <c r="K30" s="53"/>
+      <c r="L30" s="52"/>
+      <c r="M30" s="51"/>
+      <c r="N30" s="50"/>
+      <c r="O30" s="50"/>
+      <c r="P30" s="50"/>
+      <c r="Q30" s="51"/>
+      <c r="R30" s="52"/>
+      <c r="S30" s="50"/>
       <c r="T30" s="47"/>
-      <c r="U30" s="51"/>
-      <c r="V30" s="51">
+      <c r="U30" s="50"/>
+      <c r="V30" s="93">
         <v>4</v>
       </c>
-      <c r="W30" s="52"/>
-      <c r="X30" s="53"/>
-      <c r="Y30" s="51"/>
-      <c r="Z30" s="47"/>
-      <c r="AA30" s="51"/>
-      <c r="AB30" s="52"/>
-      <c r="AC30" s="53"/>
-      <c r="AD30" s="51"/>
-      <c r="AE30" s="69"/>
-      <c r="AF30" s="72"/>
+      <c r="W30" s="51"/>
+      <c r="X30" s="52"/>
+      <c r="Y30" s="81"/>
+      <c r="Z30" s="83"/>
+      <c r="AA30" s="81"/>
+      <c r="AB30" s="51"/>
+      <c r="AC30" s="52"/>
+      <c r="AD30" s="50"/>
+      <c r="AE30" s="68"/>
+      <c r="AF30" s="70"/>
       <c r="AG30" s="27"/>
       <c r="AH30" s="27"/>
       <c r="AI30" s="27"/>
@@ -3793,20 +3862,20 @@
       <c r="V31" s="30"/>
       <c r="W31" s="25"/>
       <c r="X31" s="25"/>
-      <c r="Y31" s="25"/>
-      <c r="Z31" s="25"/>
-      <c r="AA31" s="25"/>
+      <c r="Y31" s="80"/>
+      <c r="Z31" s="80"/>
+      <c r="AA31" s="80"/>
       <c r="AB31" s="25"/>
       <c r="AC31" s="25"/>
       <c r="AD31" s="25"/>
       <c r="AE31" s="26"/>
-      <c r="AF31" s="72"/>
+      <c r="AF31" s="70"/>
     </row>
     <row r="32" spans="1:42" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="36">
         <v>61</v>
       </c>
-      <c r="B32" s="59" t="s">
+      <c r="B32" s="58" t="s">
         <v>32</v>
       </c>
       <c r="C32" s="47"/>
@@ -3821,29 +3890,29 @@
       <c r="G32" s="47"/>
       <c r="H32" s="47"/>
       <c r="I32" s="48"/>
-      <c r="J32" s="54"/>
-      <c r="K32" s="54"/>
-      <c r="L32" s="53"/>
-      <c r="M32" s="52"/>
-      <c r="N32" s="51"/>
-      <c r="O32" s="51"/>
-      <c r="P32" s="51"/>
-      <c r="Q32" s="52"/>
-      <c r="R32" s="53"/>
-      <c r="S32" s="51"/>
+      <c r="J32" s="53"/>
+      <c r="K32" s="53"/>
+      <c r="L32" s="52"/>
+      <c r="M32" s="51"/>
+      <c r="N32" s="50"/>
+      <c r="O32" s="50"/>
+      <c r="P32" s="50"/>
+      <c r="Q32" s="51"/>
+      <c r="R32" s="52"/>
+      <c r="S32" s="50"/>
       <c r="T32" s="47"/>
-      <c r="U32" s="51"/>
-      <c r="V32" s="51"/>
-      <c r="W32" s="52"/>
-      <c r="X32" s="53"/>
-      <c r="Y32" s="51"/>
-      <c r="Z32" s="47"/>
-      <c r="AA32" s="51"/>
-      <c r="AB32" s="52"/>
-      <c r="AC32" s="53"/>
-      <c r="AD32" s="56"/>
-      <c r="AE32" s="69"/>
-      <c r="AF32" s="72"/>
+      <c r="U32" s="50"/>
+      <c r="V32" s="91"/>
+      <c r="W32" s="51"/>
+      <c r="X32" s="52"/>
+      <c r="Y32" s="81"/>
+      <c r="Z32" s="83"/>
+      <c r="AA32" s="81"/>
+      <c r="AB32" s="51"/>
+      <c r="AC32" s="52"/>
+      <c r="AD32" s="55"/>
+      <c r="AE32" s="68"/>
+      <c r="AF32" s="70"/>
       <c r="AG32" s="27"/>
       <c r="AH32" s="27"/>
       <c r="AI32" s="27"/>
@@ -3859,7 +3928,7 @@
       <c r="A33" s="36">
         <v>62</v>
       </c>
-      <c r="B33" s="59" t="s">
+      <c r="B33" s="58" t="s">
         <v>29</v>
       </c>
       <c r="C33" s="47"/>
@@ -3874,31 +3943,31 @@
       <c r="G33" s="47"/>
       <c r="H33" s="47"/>
       <c r="I33" s="48"/>
-      <c r="J33" s="54"/>
-      <c r="K33" s="54"/>
-      <c r="L33" s="53"/>
-      <c r="M33" s="52"/>
-      <c r="N33" s="51"/>
-      <c r="O33" s="51"/>
-      <c r="P33" s="51"/>
-      <c r="Q33" s="52"/>
-      <c r="R33" s="53"/>
-      <c r="S33" s="51"/>
+      <c r="J33" s="53"/>
+      <c r="K33" s="53"/>
+      <c r="L33" s="52"/>
+      <c r="M33" s="51"/>
+      <c r="N33" s="50"/>
+      <c r="O33" s="50"/>
+      <c r="P33" s="50"/>
+      <c r="Q33" s="51"/>
+      <c r="R33" s="52"/>
+      <c r="S33" s="50"/>
       <c r="T33" s="47"/>
-      <c r="U33" s="51"/>
-      <c r="V33" s="51"/>
-      <c r="W33" s="52"/>
-      <c r="X33" s="53"/>
-      <c r="Y33" s="51"/>
-      <c r="Z33" s="47"/>
-      <c r="AA33" s="75">
+      <c r="U33" s="50"/>
+      <c r="V33" s="91"/>
+      <c r="W33" s="51"/>
+      <c r="X33" s="52"/>
+      <c r="Y33" s="81"/>
+      <c r="Z33" s="83"/>
+      <c r="AA33" s="84">
         <v>2</v>
       </c>
-      <c r="AB33" s="52"/>
-      <c r="AC33" s="53"/>
-      <c r="AD33" s="61"/>
-      <c r="AE33" s="69"/>
-      <c r="AF33" s="72"/>
+      <c r="AB33" s="51"/>
+      <c r="AC33" s="52"/>
+      <c r="AD33" s="60"/>
+      <c r="AE33" s="68"/>
+      <c r="AF33" s="70"/>
       <c r="AG33" s="27"/>
       <c r="AH33" s="27"/>
       <c r="AI33" s="27"/>
@@ -3917,23 +3986,23 @@
       </c>
       <c r="C34" s="25">
         <f>SUM(C5+C11+C16+C25+C28+C31)</f>
-        <v>52.5</v>
+        <v>58.5</v>
       </c>
       <c r="D34" s="25">
         <f>SUM(D31+D28+D25+D16+D11+D5)</f>
-        <v>73.25</v>
+        <v>83.75</v>
       </c>
       <c r="E34" s="25"/>
       <c r="F34" s="25"/>
       <c r="G34" s="25"/>
       <c r="H34" s="25"/>
-      <c r="I34" s="62"/>
-      <c r="J34" s="63"/>
-      <c r="K34" s="64">
+      <c r="I34" s="61"/>
+      <c r="J34" s="62"/>
+      <c r="K34" s="63">
         <f>SUM(K6:K33)</f>
         <v>1</v>
       </c>
-      <c r="L34" s="65">
+      <c r="L34" s="64">
         <f>SUM(L5:L33)</f>
         <v>0</v>
       </c>
@@ -3941,90 +4010,90 @@
         <f>SUM(M5:M33)</f>
         <v>0</v>
       </c>
-      <c r="N34" s="65">
+      <c r="N34" s="88">
         <f>SUM(N5:N33)</f>
         <v>7.8</v>
       </c>
-      <c r="O34" s="65">
+      <c r="O34" s="88">
         <f>SUM(O5:O33)</f>
         <v>7.5</v>
       </c>
-      <c r="P34" s="65">
+      <c r="P34" s="88">
         <f t="shared" ref="P34:Z34" si="1">SUM(P5:P33)</f>
         <v>7</v>
       </c>
-      <c r="Q34" s="65">
+      <c r="Q34" s="88">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R34" s="25">
+      <c r="R34" s="80">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S34" s="65">
+      <c r="S34" s="88">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="T34" s="25">
+      <c r="T34" s="80">
         <f t="shared" si="1"/>
         <v>7.2</v>
       </c>
-      <c r="U34" s="65">
+      <c r="U34" s="88">
         <f t="shared" si="1"/>
         <v>7.25</v>
       </c>
-      <c r="V34" s="65">
-        <v>1</v>
-      </c>
-      <c r="W34" s="65">
+      <c r="V34" s="88">
+        <v>4</v>
+      </c>
+      <c r="W34" s="88">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="X34" s="25">
+      <c r="X34" s="80">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y34" s="65">
+      <c r="Y34" s="88">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="Z34" s="25">
+      <c r="Z34" s="80">
         <f t="shared" si="1"/>
         <v>7.5</v>
       </c>
-      <c r="AA34" s="65">
+      <c r="AA34" s="88">
         <f>SUM(AA5:AA33)</f>
         <v>7.5</v>
       </c>
-      <c r="AB34" s="65">
+      <c r="AB34" s="88">
         <f>SUM(AB5:AB33)</f>
         <v>0</v>
       </c>
-      <c r="AC34" s="25">
+      <c r="AC34" s="80">
         <f>SUM(AC5:AC33)</f>
         <v>0</v>
       </c>
-      <c r="AD34" s="65">
+      <c r="AD34" s="88">
         <f>SUM(AD5:AD33)</f>
-        <v>5.5</v>
-      </c>
-      <c r="AE34" s="26">
+        <v>7</v>
+      </c>
+      <c r="AE34" s="89">
         <f>SUM(AE5:AE33)</f>
-        <v>0</v>
-      </c>
-      <c r="AF34" s="73"/>
+        <v>6</v>
+      </c>
+      <c r="AF34" s="71"/>
     </row>
     <row r="35" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="16"/>
-      <c r="B35" s="85"/>
-      <c r="C35" s="85"/>
-      <c r="D35" s="85"/>
-      <c r="E35" s="85"/>
-      <c r="F35" s="85"/>
-      <c r="G35" s="85"/>
-      <c r="H35" s="85"/>
-      <c r="I35" s="85"/>
-      <c r="J35" s="85"/>
+      <c r="B35" s="98"/>
+      <c r="C35" s="98"/>
+      <c r="D35" s="98"/>
+      <c r="E35" s="98"/>
+      <c r="F35" s="98"/>
+      <c r="G35" s="98"/>
+      <c r="H35" s="98"/>
+      <c r="I35" s="98"/>
+      <c r="J35" s="98"/>
       <c r="K35" s="24"/>
       <c r="AG35" s="28"/>
       <c r="AH35" s="28"/>
@@ -4051,30 +4120,30 @@
       <c r="I36" s="7"/>
       <c r="J36" s="7"/>
       <c r="K36" s="7"/>
-      <c r="L36" s="83"/>
-      <c r="M36" s="84"/>
-      <c r="N36" s="84"/>
-      <c r="O36" s="84"/>
-      <c r="P36" s="84"/>
-      <c r="Q36" s="84"/>
-      <c r="R36" s="84"/>
-      <c r="S36" s="84"/>
-      <c r="T36" s="84"/>
-      <c r="U36" s="84"/>
-      <c r="V36" s="84"/>
-      <c r="W36" s="84"/>
-      <c r="X36" s="84"/>
-      <c r="Y36" s="84"/>
-      <c r="Z36" s="84"/>
-      <c r="AA36" s="84"/>
-      <c r="AB36" s="84"/>
-      <c r="AC36" s="84"/>
-      <c r="AD36" s="84"/>
-      <c r="AE36" s="84"/>
-      <c r="AF36" s="84"/>
+      <c r="L36" s="96"/>
+      <c r="M36" s="97"/>
+      <c r="N36" s="97"/>
+      <c r="O36" s="97"/>
+      <c r="P36" s="97"/>
+      <c r="Q36" s="97"/>
+      <c r="R36" s="97"/>
+      <c r="S36" s="97"/>
+      <c r="T36" s="97"/>
+      <c r="U36" s="97"/>
+      <c r="V36" s="97"/>
+      <c r="W36" s="97"/>
+      <c r="X36" s="97"/>
+      <c r="Y36" s="97"/>
+      <c r="Z36" s="97"/>
+      <c r="AA36" s="97"/>
+      <c r="AB36" s="97"/>
+      <c r="AC36" s="97"/>
+      <c r="AD36" s="97"/>
+      <c r="AE36" s="97"/>
+      <c r="AF36" s="97"/>
     </row>
     <row r="37" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="76" t="s">
+      <c r="A37" s="73" t="s">
         <v>49</v>
       </c>
       <c r="B37" s="6" t="s">
@@ -4089,30 +4158,30 @@
       <c r="I37" s="9"/>
       <c r="J37" s="9"/>
       <c r="K37" s="9"/>
-      <c r="L37" s="82"/>
-      <c r="M37" s="82"/>
-      <c r="N37" s="82"/>
-      <c r="O37" s="82"/>
-      <c r="P37" s="82"/>
-      <c r="Q37" s="82"/>
-      <c r="R37" s="82"/>
-      <c r="S37" s="82"/>
-      <c r="T37" s="82"/>
-      <c r="U37" s="82"/>
-      <c r="V37" s="82"/>
-      <c r="W37" s="82"/>
-      <c r="X37" s="82"/>
-      <c r="Y37" s="82"/>
-      <c r="Z37" s="82"/>
-      <c r="AA37" s="82"/>
-      <c r="AB37" s="82"/>
-      <c r="AC37" s="82"/>
-      <c r="AD37" s="82"/>
-      <c r="AE37" s="82"/>
-      <c r="AF37" s="82"/>
+      <c r="L37" s="95"/>
+      <c r="M37" s="95"/>
+      <c r="N37" s="95"/>
+      <c r="O37" s="95"/>
+      <c r="P37" s="95"/>
+      <c r="Q37" s="95"/>
+      <c r="R37" s="95"/>
+      <c r="S37" s="95"/>
+      <c r="T37" s="95"/>
+      <c r="U37" s="95"/>
+      <c r="V37" s="95"/>
+      <c r="W37" s="95"/>
+      <c r="X37" s="95"/>
+      <c r="Y37" s="95"/>
+      <c r="Z37" s="95"/>
+      <c r="AA37" s="95"/>
+      <c r="AB37" s="95"/>
+      <c r="AC37" s="95"/>
+      <c r="AD37" s="95"/>
+      <c r="AE37" s="95"/>
+      <c r="AF37" s="95"/>
     </row>
     <row r="38" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="77"/>
+      <c r="A38" s="74"/>
       <c r="B38" s="6" t="s">
         <v>51</v>
       </c>
@@ -4125,31 +4194,33 @@
       <c r="I38" s="9"/>
       <c r="J38" s="9"/>
       <c r="K38" s="9"/>
-      <c r="L38" s="82"/>
-      <c r="M38" s="82"/>
-      <c r="N38" s="82"/>
-      <c r="O38" s="82"/>
-      <c r="P38" s="82"/>
-      <c r="Q38" s="82"/>
-      <c r="R38" s="82"/>
-      <c r="S38" s="82"/>
-      <c r="T38" s="82"/>
-      <c r="U38" s="82"/>
-      <c r="V38" s="82"/>
-      <c r="W38" s="82"/>
-      <c r="X38" s="82"/>
-      <c r="Y38" s="82"/>
-      <c r="Z38" s="82"/>
-      <c r="AA38" s="82"/>
-      <c r="AB38" s="82"/>
-      <c r="AC38" s="82"/>
-      <c r="AD38" s="82"/>
-      <c r="AE38" s="82"/>
-      <c r="AF38" s="82"/>
+      <c r="L38" s="95"/>
+      <c r="M38" s="95"/>
+      <c r="N38" s="95"/>
+      <c r="O38" s="95"/>
+      <c r="P38" s="95"/>
+      <c r="Q38" s="95"/>
+      <c r="R38" s="95"/>
+      <c r="S38" s="95"/>
+      <c r="T38" s="95"/>
+      <c r="U38" s="95"/>
+      <c r="V38" s="95"/>
+      <c r="W38" s="95"/>
+      <c r="X38" s="95"/>
+      <c r="Y38" s="95"/>
+      <c r="Z38" s="95"/>
+      <c r="AA38" s="95"/>
+      <c r="AB38" s="95"/>
+      <c r="AC38" s="95"/>
+      <c r="AD38" s="95"/>
+      <c r="AE38" s="95"/>
+      <c r="AF38" s="95"/>
     </row>
     <row r="39" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="11"/>
-      <c r="B39" s="9"/>
+      <c r="A39" s="109"/>
+      <c r="B39" s="110" t="s">
+        <v>55</v>
+      </c>
       <c r="J39" s="5"/>
       <c r="K39" s="5"/>
     </row>
@@ -4206,8 +4277,8 @@
   </sheetPr>
   <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A33"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4219,20 +4290,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="91"/>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
-      <c r="G1" s="91"/>
-      <c r="H1" s="91"/>
-      <c r="I1" s="91"/>
-      <c r="J1" s="91"/>
-      <c r="K1" s="91"/>
-      <c r="L1" s="91"/>
-      <c r="M1" s="91"/>
-      <c r="N1" s="91"/>
+      <c r="A1" s="104"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
+      <c r="D1" s="104"/>
+      <c r="E1" s="104"/>
+      <c r="F1" s="104"/>
+      <c r="G1" s="104"/>
+      <c r="H1" s="104"/>
+      <c r="I1" s="104"/>
+      <c r="J1" s="104"/>
+      <c r="K1" s="104"/>
+      <c r="L1" s="104"/>
+      <c r="M1" s="104"/>
+      <c r="N1" s="104"/>
     </row>
     <row r="2" spans="1:14" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="17"/>
@@ -4435,7 +4506,7 @@
       </c>
       <c r="B21" s="18">
         <f>Zeitplanung!AD34</f>
-        <v>5.5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4445,7 +4516,7 @@
       </c>
       <c r="B22" s="18">
         <f>Zeitplanung!AE34</f>
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4561,10 +4632,10 @@
     <row r="34" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="36" spans="1:4" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="92" t="s">
+      <c r="A36" s="105" t="s">
         <v>20</v>
       </c>
-      <c r="B36" s="93"/>
+      <c r="B36" s="106"/>
       <c r="C36" s="3" t="s">
         <v>21</v>
       </c>
@@ -4573,24 +4644,24 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="89" t="s">
+      <c r="A37" s="102" t="s">
         <v>10</v>
       </c>
-      <c r="B37" s="90"/>
+      <c r="B37" s="103"/>
       <c r="C37" s="18">
         <f>Zeitplanung!C5</f>
         <v>16.3</v>
       </c>
       <c r="D37" s="18">
         <f>Zeitplanung!D5</f>
-        <v>17.25</v>
+        <v>19.75</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="94" t="s">
+      <c r="A38" s="107" t="s">
         <v>13</v>
       </c>
-      <c r="B38" s="95"/>
+      <c r="B38" s="108"/>
       <c r="C38" s="18">
         <f>Zeitplanung!C11</f>
         <v>2.7</v>
@@ -4601,55 +4672,54 @@
       </c>
     </row>
     <row r="39" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="89" t="s">
+      <c r="A39" s="102" t="s">
         <v>9</v>
       </c>
-      <c r="B39" s="90"/>
+      <c r="B39" s="103"/>
       <c r="C39" s="18">
         <f>Zeitplanung!C16</f>
         <v>22.5</v>
       </c>
       <c r="D39" s="18">
         <f>Zeitplanung!D16</f>
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="94" t="s">
+      <c r="A40" s="107" t="s">
         <v>7</v>
       </c>
-      <c r="B40" s="95"/>
+      <c r="B40" s="108"/>
       <c r="C40" s="18">
         <f>Zeitplanung!C25</f>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D40" s="18">
         <f>Zeitplanung!D25</f>
-        <v>19.5</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="89" t="s">
+      <c r="A41" s="102" t="s">
         <v>11</v>
       </c>
-      <c r="B41" s="90"/>
+      <c r="B41" s="103"/>
       <c r="C41" s="18">
         <f>Zeitplanung!C28</f>
         <v>6</v>
       </c>
       <c r="D41" s="18">
         <f>Zeitplanung!D28</f>
-        <v>1.5</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="89" t="s">
+      <c r="A42" s="102" t="s">
         <v>8</v>
       </c>
-      <c r="B42" s="90"/>
+      <c r="B42" s="103"/>
       <c r="C42" s="18">
-        <f>Zeitplanung!C31</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D42" s="18">
         <f>Zeitplanung!D31</f>

</xml_diff>